<commit_message>
adding tables to db/refactoring
</commit_message>
<xml_diff>
--- a/timeLog.xlsx
+++ b/timeLog.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="9048" xr2:uid="{92B6C3AA-AEFB-4873-AE11-A3A4A45A232C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="9045"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>Activity</t>
   </si>
@@ -66,12 +66,21 @@
   </si>
   <si>
     <t>Finished DaoTests, worked on Result and Index jsps</t>
+  </si>
+  <si>
+    <t>Generic Dao/Testing</t>
+  </si>
+  <si>
+    <t>Fixing tests/DB</t>
+  </si>
+  <si>
+    <t>AWS Setup / First Deploy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
@@ -423,24 +432,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FF94675-7E9B-416B-8326-D84FD13B322B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.44140625" customWidth="1"/>
-    <col min="2" max="2" width="24.44140625" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -460,7 +469,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -474,7 +483,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -489,7 +498,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -504,7 +513,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -519,7 +528,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -540,7 +549,7 @@
         <v>15.83</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -561,7 +570,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -582,7 +591,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -597,7 +606,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
@@ -612,7 +621,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>43142</v>
       </c>
@@ -627,7 +636,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>43143</v>
       </c>
@@ -642,7 +651,7 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>43144</v>
       </c>
@@ -657,7 +666,7 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>43149</v>
       </c>
@@ -672,81 +681,108 @@
         <v>37.5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E15" s="2"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>43152</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="2">
+        <v>2</v>
+      </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E16" s="2"/>
+        <v>39.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>43153</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="2">
+        <v>2</v>
+      </c>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E17" s="2"/>
+        <v>41.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>43157</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="2">
+        <v>6</v>
+      </c>
       <c r="F17">
         <f t="shared" si="0"/>
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="18" spans="5:6" x14ac:dyDescent="0.3">
+        <v>47.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>43158</v>
+      </c>
       <c r="E18" s="2"/>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.3">
+        <v>47.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E19" s="2"/>
       <c r="F19">
         <f t="shared" si="0"/>
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="20" spans="5:6" x14ac:dyDescent="0.3">
+        <v>47.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E20" s="2"/>
       <c r="F20">
         <f t="shared" si="0"/>
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="21" spans="5:6" x14ac:dyDescent="0.3">
+        <v>47.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E21" s="2"/>
       <c r="F21">
         <f t="shared" si="0"/>
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="22" spans="5:6" x14ac:dyDescent="0.3">
+        <v>47.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E22" s="2"/>
       <c r="F22">
         <f t="shared" si="0"/>
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="23" spans="5:6" x14ac:dyDescent="0.3">
+        <v>47.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E23" s="2"/>
       <c r="F23">
         <f t="shared" si="0"/>
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="24" spans="5:6" x14ac:dyDescent="0.3">
+        <v>47.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E24" s="2"/>
       <c r="F24">
         <f t="shared" si="0"/>
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="25" spans="5:6" x14ac:dyDescent="0.3">
+        <v>47.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E25" s="2"/>
       <c r="F25">
         <f t="shared" si="0"/>
-        <v>37.5</v>
+        <v>47.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>